<commit_message>
Includes Suporte_Relatorio.xlsx in worktree
</commit_message>
<xml_diff>
--- a/Suporte_Relatorio.xlsx
+++ b/Suporte_Relatorio.xlsx
@@ -4055,8 +4055,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010029DFE9A47EDBBA4C9642CECEC7AB5212" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8f2c6ae4a50a8b148bb7565151eccd01">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685e8f7b-ce85-439b-962f-3948db74e463" xmlns:ns3="9968dc3e-a1f3-41f5-b998-9e98f3d19f76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="182854d0ea7c01653fabf173265a5b93" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010029DFE9A47EDBBA4C9642CECEC7AB5212" ma:contentTypeVersion="15" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="7328ff878a8f4dae18a74358abfdf779">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="685e8f7b-ce85-439b-962f-3948db74e463" xmlns:ns3="9968dc3e-a1f3-41f5-b998-9e98f3d19f76" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d504a395b7aacda9b17f0d85dc998159" ns2:_="" ns3:_="">
     <xsd:import namespace="685e8f7b-ce85-439b-962f-3948db74e463"/>
     <xsd:import namespace="9968dc3e-a1f3-41f5-b998-9e98f3d19f76"/>
     <xsd:element name="properties">
@@ -4109,7 +4109,7 @@
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d8ce33f6-733d-4e00-8801-5e8569691fea" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="15" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Marcações de imagem" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="d8ce33f6-733d-4e00-8801-5e8569691fea" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
       <xsd:complexType>
         <xsd:sequence>
           <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
@@ -4152,7 +4152,7 @@
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="9968dc3e-a1f3-41f5-b998-9e98f3d19f76" elementFormDefault="qualified">
     <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
+    <xsd:element name="SharedWithUsers" ma:index="12" nillable="true" ma:displayName="Compartilhado com" ma:internalName="SharedWithUsers" ma:readOnly="true">
       <xsd:complexType>
         <xsd:complexContent>
           <xsd:extension base="dms:UserMulti">
@@ -4171,7 +4171,7 @@
         </xsd:complexContent>
       </xsd:complexType>
     </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
+    <xsd:element name="SharedWithDetails" ma:index="13" nillable="true" ma:displayName="Detalhes de Compartilhado Com" ma:internalName="SharedWithDetails" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note">
           <xsd:maxLength value="255"/>
@@ -4199,8 +4199,8 @@
         <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
+        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Tipo de Conteúdo"/>
+        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Título"/>
         <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
         <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
         <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
@@ -4317,22 +4317,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BA1717C-B4B5-41B3-9092-3632DE0736F1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="685e8f7b-ce85-439b-962f-3948db74e463"/>
-    <ds:schemaRef ds:uri="9968dc3e-a1f3-41f5-b998-9e98f3d19f76"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ADBD3FE2-B07C-4FEE-BF76-FF710C6DD52A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Mudança na SUPORTE 2
</commit_message>
<xml_diff>
--- a/Suporte_Relatorio.xlsx
+++ b/Suporte_Relatorio.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ekhofo-my.sharepoint.com/personal/rafael_astolfi_ekhofo_com/Documents/Desktop/relatorio_mensal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="366" documentId="8_{96E81CA7-990A-4452-BFD6-B12F48A36CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21078098-A8E9-43A6-8D97-BE998906A0BF}"/>
+  <xr:revisionPtr revIDLastSave="375" documentId="8_{96E81CA7-990A-4452-BFD6-B12F48A36CD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0B63BC5C-7595-46D1-A722-0A8546F2553F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="7" xr2:uid="{D83840C6-8BB1-4146-989F-64A28F905889}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="2" activeTab="5" xr2:uid="{D83840C6-8BB1-4146-989F-64A28F905889}"/>
   </bookViews>
   <sheets>
     <sheet name="classes" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1017" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="224">
   <si>
     <t>Alternativos</t>
   </si>
@@ -2004,9 +2004,9 @@
   <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C18" sqref="C17:C18"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E75"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3298,18 +3298,38 @@
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="3"/>
-      <c r="B76" s="3"/>
-      <c r="C76" s="3"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="6"/>
+      <c r="A76" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1010</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="6">
+        <v>45373</v>
+      </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-      <c r="C77" s="3"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="6"/>
+      <c r="A77" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="3">
+        <v>2037</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="6">
+        <v>45509</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{492A2C00-84DF-4782-A4AE-C9B5D9D242D2}"/>
@@ -3323,12 +3343,12 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C18" sqref="C17:C18"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E59"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3480,36 +3500,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3">
-        <v>1010</v>
+        <v>1040</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6">
-        <v>45373</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3">
-        <v>1040</v>
+        <v>1096</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="6">
-        <v>45435</v>
+        <v>44942</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3517,33 +3537,33 @@
         <v>125</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="6">
-        <v>44942</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3">
-        <v>1095</v>
+        <v>22365</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="6">
-        <v>44949</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3551,16 +3571,16 @@
         <v>115</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3">
-        <v>22365</v>
+        <v>1089</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="6">
-        <v>45195</v>
+        <v>45202</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3568,16 +3588,16 @@
         <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3">
-        <v>1089</v>
+        <v>30022</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="6">
-        <v>45202</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3585,10 +3605,10 @@
         <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3">
-        <v>30022</v>
+        <v>1091</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>23</v>
@@ -3602,16 +3622,16 @@
         <v>115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3">
-        <v>1091</v>
+        <v>22368</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="6">
-        <v>45392</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3619,16 +3639,16 @@
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3">
-        <v>22368</v>
+        <v>1090</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="6">
-        <v>45195</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,16 +3656,16 @@
         <v>115</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3">
-        <v>1090</v>
+        <v>22353</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="6">
-        <v>45443</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3653,16 +3673,16 @@
         <v>115</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3">
-        <v>22353</v>
+        <v>40010</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="6">
-        <v>45195</v>
+        <v>43074</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3670,33 +3690,33 @@
         <v>115</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3">
-        <v>40010</v>
+        <v>22801</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="6">
-        <v>43074</v>
+        <v>45294</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C21" s="3">
-        <v>22801</v>
+        <v>21223</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="6">
-        <v>45294</v>
+        <v>43069</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,10 +3724,10 @@
         <v>135</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C22" s="3">
-        <v>21223</v>
+        <v>40006</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
@@ -3718,36 +3738,36 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3">
-        <v>40006</v>
+        <v>50007</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="6">
-        <v>43069</v>
+        <v>45200</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C24" s="3">
-        <v>50007</v>
+        <v>1031</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="6">
-        <v>45200</v>
+        <v>45077</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,10 +3775,10 @@
         <v>129</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="C25" s="3">
-        <v>1031</v>
+        <v>3006</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>23</v>
@@ -3769,87 +3789,87 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="C26" s="3">
-        <v>3006</v>
+        <v>50042</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="6">
-        <v>45077</v>
+        <v>45170</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C27" s="3">
-        <v>50042</v>
+        <v>1043</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="6">
-        <v>45170</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="C28" s="3">
-        <v>1043</v>
+        <v>1013</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="6">
-        <v>45436</v>
+        <v>45117</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3">
-        <v>1013</v>
+        <v>30002</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="6">
-        <v>45117</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C30" s="3">
-        <v>30002</v>
+        <v>1018</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="6">
-        <v>45306</v>
+        <v>45202</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,10 +3877,10 @@
         <v>126</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C31" s="3">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>23</v>
@@ -3871,36 +3891,36 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3">
-        <v>1020</v>
+        <v>50034</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="6">
-        <v>45202</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3">
-        <v>50034</v>
+        <v>40005</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="6">
-        <v>45210</v>
+        <v>42375</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3908,10 +3928,10 @@
         <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="C34" s="3">
-        <v>40005</v>
+        <v>21220</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>23</v>
@@ -3922,36 +3942,36 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3">
-        <v>21220</v>
+        <v>1036</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E35" s="6">
-        <v>42375</v>
+        <v>44712</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C36" s="3">
-        <v>1036</v>
+        <v>21217</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="6">
-        <v>44712</v>
+        <v>43840</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3959,10 +3979,10 @@
         <v>134</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="C37" s="3">
-        <v>21217</v>
+        <v>40001</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>23</v>
@@ -3973,36 +3993,36 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3">
-        <v>40001</v>
+        <v>1006</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="6">
-        <v>43840</v>
+        <v>45351</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C39" s="3">
-        <v>1006</v>
+        <v>40011</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="6">
-        <v>45351</v>
+        <v>42737</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -4010,10 +4030,10 @@
         <v>118</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="C40" s="3">
-        <v>40011</v>
+        <v>21226</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>23</v>
@@ -4024,19 +4044,19 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C41" s="3">
-        <v>21226</v>
+        <v>1110</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E41" s="6">
-        <v>42737</v>
+        <v>42954</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -4044,10 +4064,10 @@
         <v>146</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3">
-        <v>1110</v>
+        <v>40013</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>23</v>
@@ -4061,84 +4081,84 @@
         <v>146</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C43" s="3">
-        <v>40013</v>
+        <v>21208</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E43" s="6">
-        <v>42954</v>
+        <v>43007</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C44" s="3">
-        <v>21208</v>
+        <v>1116</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="6">
-        <v>43007</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C45" s="3">
-        <v>1116</v>
+        <v>1087</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E45" s="6">
-        <v>45471</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C46" s="3">
-        <v>1087</v>
+        <v>1117</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="6">
-        <v>45443</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3">
-        <v>1117</v>
+        <v>22582</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="6">
-        <v>45474</v>
+        <v>45383</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -4146,7 +4166,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="3">
         <v>22582</v>
@@ -4160,19 +4180,19 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="C49" s="3">
-        <v>22582</v>
+        <v>1125</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E49" s="6">
-        <v>45383</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,10 +4200,10 @@
         <v>200</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>23</v>
@@ -4197,10 +4217,10 @@
         <v>200</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C51" s="3">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>23</v>
@@ -4214,10 +4234,10 @@
         <v>200</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C52" s="3">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>23</v>
@@ -4231,10 +4251,10 @@
         <v>200</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" s="3">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>23</v>
@@ -4248,10 +4268,10 @@
         <v>200</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C54" s="3">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>23</v>
@@ -4265,10 +4285,10 @@
         <v>200</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C55" s="3">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>23</v>
@@ -4282,10 +4302,10 @@
         <v>200</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="C56" s="3">
-        <v>1114</v>
+        <v>1119</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>23</v>
@@ -4296,19 +4316,19 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="C57" s="3">
-        <v>1119</v>
+        <v>1046</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E57" s="6">
-        <v>45471</v>
+        <v>44837</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,10 +4336,10 @@
         <v>217</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C58" s="3">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>23</v>
@@ -4329,24 +4349,7 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C59" s="3">
-        <v>1045</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="6">
-        <v>44837</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E60" s="6"/>
+      <c r="E59" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{6EEBEAB0-4E16-4581-8A08-39CF6708FA50}"/>
@@ -4358,12 +4361,12 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73CF0191-5EAE-4B06-B5C1-13D30342DEF8}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B12" sqref="B12"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:E77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5722,6 +5725,40 @@
         <v>44837</v>
       </c>
     </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1010</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E76" s="6">
+        <v>45373</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="3">
+        <v>2037</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E77" s="6">
+        <v>45509</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:D49" xr:uid="{FDD9564B-AAE5-4B8B-854B-0D27C6086BCC}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5731,12 +5768,12 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B548D8A-88F4-48BF-8DA9-473567F1EB6D}">
-  <dimension ref="A1:E151"/>
+  <dimension ref="A1:E150"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B12" sqref="B12"/>
-      <selection pane="bottomLeft" activeCell="J6" sqref="J6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5886,36 +5923,36 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>76</v>
+        <v>97</v>
       </c>
       <c r="C9" s="3">
-        <v>1010</v>
+        <v>1040</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E9" s="6">
-        <v>45373</v>
+        <v>45435</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C10" s="3">
-        <v>1040</v>
+        <v>1096</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E10" s="6">
-        <v>45435</v>
+        <v>44942</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -5923,33 +5960,33 @@
         <v>125</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C11" s="3">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E11" s="6">
-        <v>44942</v>
+        <v>44949</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C12" s="3">
-        <v>1095</v>
+        <v>22365</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E12" s="6">
-        <v>44949</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -5957,16 +5994,16 @@
         <v>115</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C13" s="3">
-        <v>22365</v>
+        <v>1089</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="6">
-        <v>45195</v>
+        <v>45202</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -5974,16 +6011,16 @@
         <v>115</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C14" s="3">
-        <v>1089</v>
+        <v>30022</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E14" s="6">
-        <v>45202</v>
+        <v>45392</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -5991,10 +6028,10 @@
         <v>115</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="C15" s="3">
-        <v>30022</v>
+        <v>1091</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>23</v>
@@ -6008,16 +6045,16 @@
         <v>115</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C16" s="3">
-        <v>1091</v>
+        <v>22368</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E16" s="6">
-        <v>45392</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6025,16 +6062,16 @@
         <v>115</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C17" s="3">
-        <v>22368</v>
+        <v>1090</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="6">
-        <v>45195</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6042,16 +6079,16 @@
         <v>115</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="C18" s="3">
-        <v>1090</v>
+        <v>22353</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E18" s="6">
-        <v>45443</v>
+        <v>45195</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6059,16 +6096,16 @@
         <v>115</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="C19" s="3">
-        <v>22353</v>
+        <v>40010</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="6">
-        <v>45195</v>
+        <v>43074</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6076,33 +6113,33 @@
         <v>115</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C20" s="3">
-        <v>40010</v>
+        <v>22801</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E20" s="6">
-        <v>43074</v>
+        <v>45294</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>86</v>
+        <v>106</v>
       </c>
       <c r="C21" s="3">
-        <v>22801</v>
+        <v>21223</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E21" s="6">
-        <v>45294</v>
+        <v>43069</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6110,10 +6147,10 @@
         <v>135</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C22" s="3">
-        <v>21223</v>
+        <v>40006</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>23</v>
@@ -6124,36 +6161,36 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>107</v>
+        <v>48</v>
       </c>
       <c r="C23" s="3">
-        <v>40006</v>
+        <v>50007</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E23" s="6">
-        <v>43069</v>
+        <v>45200</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="C24" s="3">
-        <v>50007</v>
+        <v>1031</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E24" s="6">
-        <v>45200</v>
+        <v>45077</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -6161,10 +6198,10 @@
         <v>129</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>99</v>
+        <v>210</v>
       </c>
       <c r="C25" s="3">
-        <v>1031</v>
+        <v>3006</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>23</v>
@@ -6175,87 +6212,87 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>210</v>
+        <v>70</v>
       </c>
       <c r="C26" s="3">
-        <v>3006</v>
+        <v>50042</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E26" s="6">
-        <v>45077</v>
+        <v>45170</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="C27" s="3">
-        <v>50042</v>
+        <v>1043</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E27" s="6">
-        <v>45170</v>
+        <v>45436</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>144</v>
+        <v>75</v>
       </c>
       <c r="C28" s="3">
-        <v>1043</v>
+        <v>1013</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E28" s="6">
-        <v>45436</v>
+        <v>45117</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="C29" s="3">
-        <v>1013</v>
+        <v>30002</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E29" s="6">
-        <v>45117</v>
+        <v>45306</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="C30" s="3">
-        <v>30002</v>
+        <v>1018</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E30" s="6">
-        <v>45306</v>
+        <v>45202</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6263,10 +6300,10 @@
         <v>126</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C31" s="3">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>23</v>
@@ -6277,36 +6314,36 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="C32" s="3">
-        <v>1020</v>
+        <v>50034</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E32" s="6">
-        <v>45202</v>
+        <v>45210</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>111</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="C33" s="3">
-        <v>50034</v>
+        <v>40005</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E33" s="6">
-        <v>45210</v>
+        <v>42375</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6314,10 +6351,10 @@
         <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>52</v>
+        <v>103</v>
       </c>
       <c r="C34" s="3">
-        <v>40005</v>
+        <v>21220</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>23</v>
@@ -6328,36 +6365,36 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>52</v>
+        <v>132</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="C35" s="3">
-        <v>21220</v>
+        <v>1036</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E35" s="6">
-        <v>42375</v>
+        <v>44712</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C36" s="3">
-        <v>1036</v>
+        <v>21217</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E36" s="6">
-        <v>44712</v>
+        <v>43840</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6365,10 +6402,10 @@
         <v>134</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>45</v>
+        <v>104</v>
       </c>
       <c r="C37" s="3">
-        <v>21217</v>
+        <v>40001</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>23</v>
@@ -6379,36 +6416,36 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>104</v>
+        <v>53</v>
       </c>
       <c r="C38" s="3">
-        <v>40001</v>
+        <v>1006</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="6">
-        <v>43840</v>
+        <v>45351</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>53</v>
+        <v>78</v>
       </c>
       <c r="C39" s="3">
-        <v>1006</v>
+        <v>40011</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="6">
-        <v>45351</v>
+        <v>42737</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -6416,10 +6453,10 @@
         <v>118</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>145</v>
       </c>
       <c r="C40" s="3">
-        <v>40011</v>
+        <v>21226</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>23</v>
@@ -6430,19 +6467,19 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>118</v>
+        <v>146</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C41" s="3">
-        <v>21226</v>
+        <v>1110</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E41" s="6">
-        <v>42737</v>
+        <v>42954</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6450,10 +6487,10 @@
         <v>146</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C42" s="3">
-        <v>1110</v>
+        <v>40013</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>23</v>
@@ -6467,84 +6504,84 @@
         <v>146</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C43" s="3">
-        <v>40013</v>
+        <v>21208</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E43" s="6">
-        <v>42954</v>
+        <v>43007</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C44" s="3">
-        <v>21208</v>
+        <v>1116</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E44" s="6">
-        <v>43007</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C45" s="3">
-        <v>1116</v>
+        <v>1087</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E45" s="6">
-        <v>45471</v>
+        <v>45443</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>111</v>
+        <v>153</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C46" s="3">
-        <v>1087</v>
+        <v>1117</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E46" s="6">
-        <v>45443</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>153</v>
+        <v>111</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>154</v>
+        <v>50</v>
       </c>
       <c r="C47" s="3">
-        <v>1117</v>
+        <v>22582</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E47" s="6">
-        <v>45474</v>
+        <v>45383</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6552,7 +6589,7 @@
         <v>111</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C48" s="3">
         <v>22582</v>
@@ -6566,19 +6603,19 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>49</v>
+        <v>199</v>
       </c>
       <c r="C49" s="3">
-        <v>22582</v>
+        <v>1125</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E49" s="6">
-        <v>45383</v>
+        <v>45471</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6586,10 +6623,10 @@
         <v>200</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="C50" s="3">
-        <v>1125</v>
+        <v>1126</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>23</v>
@@ -6603,10 +6640,10 @@
         <v>200</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C51" s="3">
-        <v>1126</v>
+        <v>1118</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>23</v>
@@ -6620,10 +6657,10 @@
         <v>200</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C52" s="3">
-        <v>1118</v>
+        <v>1112</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>23</v>
@@ -6637,10 +6674,10 @@
         <v>200</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C53" s="3">
-        <v>1112</v>
+        <v>1113</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>23</v>
@@ -6654,10 +6691,10 @@
         <v>200</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="C54" s="3">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>23</v>
@@ -6671,10 +6708,10 @@
         <v>200</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C55" s="3">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>23</v>
@@ -6688,10 +6725,10 @@
         <v>200</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>206</v>
+        <v>216</v>
       </c>
       <c r="C56" s="3">
-        <v>1114</v>
+        <v>1119</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>23</v>
@@ -6702,19 +6739,19 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>216</v>
+        <v>217</v>
+      </c>
+      <c r="B57" s="6" t="s">
+        <v>219</v>
       </c>
       <c r="C57" s="3">
-        <v>1119</v>
+        <v>1046</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>23</v>
       </c>
       <c r="E57" s="6">
-        <v>45471</v>
+        <v>44837</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -6722,10 +6759,10 @@
         <v>217</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C58" s="3">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>23</v>
@@ -6735,21 +6772,9 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="C59" s="3">
-        <v>1045</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E59" s="6">
-        <v>44837</v>
-      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
+      <c r="E59" s="6"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C60" s="3"/>
@@ -7205,11 +7230,6 @@
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
       <c r="E150" s="6"/>
-    </row>
-    <row r="151" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="6"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:C56" xr:uid="{A787322A-5B17-4E1F-B960-30BFFEBBD83A}"/>

</xml_diff>